<commit_message>
prototipo di caricamento della pagina personalizzata v1
Lettura delle proprietà css da database + rendering della pagina tramite applicazione delle proprietà
</commit_message>
<xml_diff>
--- a/tabella layouts.xlsx
+++ b/tabella layouts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oirad\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\provaTesi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3E201B-B219-46B7-8FCD-6A72DD4CCAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753FD8D5-3AF8-4F87-ADE1-2994A4EA365E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E051E1CF-2EA6-4853-BFB7-5AAC7DA8918D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="30">
   <si>
     <t>tizio1</t>
   </si>
@@ -136,21 +136,6 @@
     <t>ROW</t>
   </si>
   <si>
-    <t>row1</t>
-  </si>
-  <si>
-    <t>row2</t>
-  </si>
-  <si>
-    <t>row3</t>
-  </si>
-  <si>
-    <t>row4</t>
-  </si>
-  <si>
-    <t>select col1,col2,col3,col4 from tabella where user_id=tizio1 and row=row1 mi restutisce tutta la prima riga di tizio1</t>
-  </si>
-  <si>
     <t xml:space="preserve">select col1,row from tabella where user_id=tizio1 mi restutisce tutta la prima colonna e le rispettive righe di tizio1 </t>
   </si>
   <si>
@@ -158,6 +143,9 @@
   </si>
   <si>
     <t>USER_ID(foreign key)</t>
+  </si>
+  <si>
+    <t>select col1,col2,col3,col4 from tabella where user_id=tizio1 and row=1 mi restutisce tutta la prima riga di tizio1</t>
   </si>
 </sst>
 </file>
@@ -547,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C15D8CFE-1030-4836-842B-95ECF7DABADA}">
   <dimension ref="E2:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,7 +549,7 @@
     <row r="2" spans="5:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="5:13" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="5:13" x14ac:dyDescent="0.25">
@@ -569,7 +557,7 @@
         <v>20</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>25</v>
@@ -597,8 +585,8 @@
       <c r="F13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>26</v>
+      <c r="G13" s="2">
+        <v>1</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>3</v>
@@ -620,8 +608,8 @@
       <c r="F14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>27</v>
+      <c r="G14" s="2">
+        <v>2</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>7</v>
@@ -636,7 +624,7 @@
         <v>10</v>
       </c>
       <c r="M14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="5:13" x14ac:dyDescent="0.25">
@@ -646,8 +634,8 @@
       <c r="F15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>28</v>
+      <c r="G15" s="2">
+        <v>3</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>11</v>
@@ -669,8 +657,8 @@
       <c r="F16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>29</v>
+      <c r="G16" s="2">
+        <v>4</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>15</v>
@@ -685,7 +673,7 @@
         <v>18</v>
       </c>
       <c r="M16" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="5:11" x14ac:dyDescent="0.25">
@@ -695,8 +683,8 @@
       <c r="F17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>26</v>
+      <c r="G17" s="2">
+        <v>1</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>3</v>
@@ -718,8 +706,8 @@
       <c r="F18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>27</v>
+      <c r="G18" s="2">
+        <v>2</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>7</v>
@@ -741,8 +729,8 @@
       <c r="F19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>28</v>
+      <c r="G19" s="2">
+        <v>3</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>11</v>
@@ -764,8 +752,8 @@
       <c r="F20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>29</v>
+      <c r="G20" s="2">
+        <v>4</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>15</v>
@@ -787,8 +775,8 @@
       <c r="F21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>26</v>
+      <c r="G21" s="2">
+        <v>1</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>3</v>
@@ -810,8 +798,8 @@
       <c r="F22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>27</v>
+      <c r="G22" s="2">
+        <v>2</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>7</v>
@@ -833,8 +821,8 @@
       <c r="F23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>28</v>
+      <c r="G23" s="2">
+        <v>3</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>11</v>
@@ -856,8 +844,8 @@
       <c r="F24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>29</v>
+      <c r="G24" s="2">
+        <v>4</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>15</v>

</xml_diff>